<commit_message>
Updating alignment of text in tables
</commit_message>
<xml_diff>
--- a/Tables_and_Graphs.xlsx
+++ b/Tables_and_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\university-calgary\ENSF-594\a2-comparison-of-sorting-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5121C6C3-02BC-43CB-8844-ABB249AB018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58391CC0-C117-44DC-9E77-5CC4AFC7E67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -438,49 +438,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -499,7 +456,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -510,33 +467,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -545,36 +475,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -585,20 +485,74 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -5039,9 +4993,8 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" customWidth="1"/>
+    <col min="3" max="7" width="13.77734375" style="2" customWidth="1"/>
     <col min="8" max="20" width="8.88671875" style="2" customWidth="1"/>
     <col min="21" max="16384" width="8.88671875" style="2" hidden="1"/>
   </cols>
@@ -5058,38 +5011,38 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="29" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="30">
         <v>10</v>
       </c>
       <c r="D5" s="10">
@@ -5106,209 +5059,209 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
-      <c r="C6" s="24">
+      <c r="B6" s="8"/>
+      <c r="C6" s="31">
         <v>100</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="13">
         <v>1.7670999999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="14">
         <v>1.5922000000000001</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="14">
         <v>1.601</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="15">
         <v>1.6677</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
-      <c r="C7" s="24">
+      <c r="B7" s="8"/>
+      <c r="C7" s="31">
         <v>1000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="13">
         <v>8.6206999999999994</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="14">
         <v>7.0343</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="14">
         <v>2.8795000000000002</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="15">
         <v>6.1856999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="24">
+      <c r="B8" s="8"/>
+      <c r="C8" s="31">
         <v>10000</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="13">
         <v>77.296700000000001</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="14">
         <v>33.084600000000002</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="14">
         <v>6.0928000000000004</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="15">
         <v>17.0152</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="24">
+      <c r="B9" s="8"/>
+      <c r="C9" s="31">
         <v>100000</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="13">
         <v>6339.2763999999997</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="14">
         <v>1559.2708</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="14">
         <v>20.549199999999999</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="15">
         <v>142.83420000000001</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="28"/>
-      <c r="C10" s="25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="32">
         <v>1000000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="16">
         <v>753806.39509999997</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="17">
         <v>273967.66840000002</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="17">
         <v>91.410300000000007</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="29" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="19" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="30">
         <v>10</v>
       </c>
       <c r="D23" s="10">
@@ -5325,298 +5278,300 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="27"/>
-      <c r="C24" s="24">
+      <c r="B24" s="8"/>
+      <c r="C24" s="31">
         <v>100</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="13">
         <v>2.8864000000000001</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="14">
         <v>1.4482999999999999</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="14">
         <v>1.4502999999999999</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="15">
         <v>1.3813</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="27"/>
-      <c r="C25" s="24">
+      <c r="B25" s="8"/>
+      <c r="C25" s="31">
         <v>1000</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="13">
         <v>8.8522999999999996</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="14">
         <v>5.5576999999999996</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="14">
         <v>2.9803999999999999</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="15">
         <v>2.0384000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="27"/>
-      <c r="C26" s="24">
+      <c r="B26" s="8"/>
+      <c r="C26" s="31">
         <v>10000</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="13">
         <v>150.69829999999999</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="14">
         <v>17.449200000000001</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="14">
         <v>6.3174000000000001</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="15">
         <v>4.8029000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
-      <c r="C27" s="24">
+      <c r="B27" s="8"/>
+      <c r="C27" s="31">
         <v>100000</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="13">
         <v>14663.690699999999</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="14">
         <v>742.89390000000003</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="14">
         <v>19.429600000000001</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="15">
         <v>22.835999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="28"/>
-      <c r="C28" s="25">
+      <c r="B28" s="9"/>
+      <c r="C28" s="32">
         <v>1000000</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="16">
         <v>1665448.8703999999</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="17">
         <v>86110.613400000002</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="17">
         <v>146.72309999999999</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="18">
         <v>353.56630000000001</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="13"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="29" t="s">
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="31"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="19" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="26" t="s">
+    <row r="41" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="30">
         <v>10</v>
       </c>
       <c r="D41" s="10">
         <v>1.3279000000000001</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="11">
         <v>1.3867</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F41" s="11">
         <v>1.4225000000000001</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="12">
         <v>1.4307000000000001</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="27"/>
-      <c r="C42" s="24">
+      <c r="B42" s="8"/>
+      <c r="C42" s="31">
         <v>100</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="13">
         <v>1.6232</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="14">
         <v>1.3422000000000001</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="14">
         <v>1.5330999999999999</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G42" s="15">
         <v>1.7311000000000001</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="27"/>
-      <c r="C43" s="24">
+      <c r="B43" s="8"/>
+      <c r="C43" s="31">
         <v>1000</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="13">
         <v>7.2839999999999998</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="14">
         <v>1.4282999999999999</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="14">
         <v>2.8725000000000001</v>
       </c>
-      <c r="G43" s="17">
+      <c r="G43" s="15">
         <v>7.8661000000000003</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="27"/>
-      <c r="C44" s="24">
+      <c r="B44" s="8"/>
+      <c r="C44" s="31">
         <v>10000</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="13">
         <v>28.678799999999999</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="14">
         <v>1.9876</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="14">
         <v>5.2422000000000004</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G44" s="15">
         <v>27.145600000000002</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="27"/>
-      <c r="C45" s="24">
+      <c r="B45" s="8"/>
+      <c r="C45" s="31">
         <v>100000</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="13">
         <v>1196.0227</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="14">
         <v>5.7565</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="14">
         <v>21.940999999999999</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="28"/>
-      <c r="C46" s="25">
+      <c r="B46" s="9"/>
+      <c r="C46" s="32">
         <v>1000000</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="16">
         <v>115733.3627</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="17">
         <v>10.1188</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="17">
         <v>80.877200000000002</v>
       </c>
       <c r="G46" s="18" t="s">
@@ -5624,76 +5579,76 @@
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="13"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="13"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="13"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="13"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="13"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="13"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>